<commit_message>
eau utile calculation commit
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>temperature_2m</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>ETR_PV</t>
+  </si>
+  <si>
+    <t>RDU</t>
+  </si>
+  <si>
+    <t>capacité au champs</t>
   </si>
 </sst>
 </file>
@@ -416,13 +422,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N97"/>
+  <dimension ref="A1:P97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,8 +468,14 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="2">
         <v>42144</v>
       </c>
@@ -489,10 +501,10 @@
         <v>3.336153134005934</v>
       </c>
       <c r="I2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J2">
-        <v>1.334461253602374</v>
+        <v>1.668076567002967</v>
       </c>
       <c r="K2">
         <v>575.88865542</v>
@@ -504,10 +516,16 @@
         <v>3.30773796825822</v>
       </c>
       <c r="N2">
-        <v>1.323095187303288</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>1.65386898412911</v>
+      </c>
+      <c r="O2">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P2">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="2">
         <v>42145</v>
       </c>
@@ -533,10 +551,10 @@
         <v>2.994551714646976</v>
       </c>
       <c r="I3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J3">
-        <v>1.19782068585879</v>
+        <v>1.497275857323488</v>
       </c>
       <c r="K3">
         <v>472.2116593185</v>
@@ -548,10 +566,16 @@
         <v>2.969482051511526</v>
       </c>
       <c r="N3">
-        <v>1.187792820604611</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>1.484741025755763</v>
+      </c>
+      <c r="O3">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P3">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="2">
         <v>42146</v>
       </c>
@@ -577,10 +601,10 @@
         <v>3.815373643475935</v>
       </c>
       <c r="I4">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J4">
-        <v>1.526149457390374</v>
+        <v>1.907686821737968</v>
       </c>
       <c r="K4">
         <v>575.4627022725</v>
@@ -592,10 +616,16 @@
         <v>3.782878696632072</v>
       </c>
       <c r="N4">
-        <v>1.513151478652829</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>1.891439348316036</v>
+      </c>
+      <c r="O4">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P4">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="2">
         <v>42147</v>
       </c>
@@ -621,10 +651,10 @@
         <v>2.999766468192259</v>
       </c>
       <c r="I5">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J5">
-        <v>1.199906587276904</v>
+        <v>1.49988323409613</v>
       </c>
       <c r="K5">
         <v>407.1260183805</v>
@@ -636,10 +666,16 @@
         <v>2.97502863148258</v>
       </c>
       <c r="N5">
-        <v>1.190011452593032</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>1.48751431574129</v>
+      </c>
+      <c r="O5">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P5">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="2">
         <v>42148</v>
       </c>
@@ -665,10 +701,10 @@
         <v>3.832021445568601</v>
       </c>
       <c r="I6">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J6">
-        <v>1.53280857822744</v>
+        <v>1.9160107227843</v>
       </c>
       <c r="K6">
         <v>532.6970062635</v>
@@ -680,10 +716,16 @@
         <v>3.799591069916183</v>
       </c>
       <c r="N6">
-        <v>1.519836427966473</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>1.899795534958091</v>
+      </c>
+      <c r="O6">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P6">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="2">
         <v>42149</v>
       </c>
@@ -709,10 +751,10 @@
         <v>2.458910714441926</v>
       </c>
       <c r="I7">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J7">
-        <v>0.9835642857767705</v>
+        <v>1.229455357220963</v>
       </c>
       <c r="K7">
         <v>332.8397894565</v>
@@ -724,10 +766,16 @@
         <v>2.439112426310676</v>
       </c>
       <c r="N7">
-        <v>0.9756449705242703</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>1.219556213155338</v>
+      </c>
+      <c r="O7">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P7">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="2">
         <v>42150</v>
       </c>
@@ -753,10 +801,10 @@
         <v>2.199444741166472</v>
       </c>
       <c r="I8">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J8">
-        <v>0.8797778964665888</v>
+        <v>1.099722370583236</v>
       </c>
       <c r="K8">
         <v>302.5119253545</v>
@@ -768,10 +816,16 @@
         <v>2.181962639243162</v>
       </c>
       <c r="N8">
-        <v>0.8727850556972648</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>1.090981319621581</v>
+      </c>
+      <c r="O8">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P8">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="2">
         <v>42151</v>
       </c>
@@ -797,10 +851,10 @@
         <v>4.229318654521739</v>
       </c>
       <c r="I9">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J9">
-        <v>1.691727461808696</v>
+        <v>2.11465932726087</v>
       </c>
       <c r="K9">
         <v>597.2715034245</v>
@@ -812,10 +866,16 @@
         <v>4.193193652619588</v>
       </c>
       <c r="N9">
-        <v>1.677277461047835</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>2.096596826309794</v>
+      </c>
+      <c r="O9">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P9">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="2">
         <v>42152</v>
       </c>
@@ -841,10 +901,10 @@
         <v>3.49400604184381</v>
       </c>
       <c r="I10">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J10">
-        <v>1.397602416737524</v>
+        <v>1.747003020921905</v>
       </c>
       <c r="K10">
         <v>481.4122473045</v>
@@ -856,10 +916,16 @@
         <v>3.464701893738532</v>
       </c>
       <c r="N10">
-        <v>1.385880757495413</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>1.732350946869266</v>
+      </c>
+      <c r="O10">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P10">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="2">
         <v>42153</v>
       </c>
@@ -885,10 +951,10 @@
         <v>2.352145049669065</v>
       </c>
       <c r="I11">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J11">
-        <v>0.9408580198676258</v>
+        <v>1.176072524834532</v>
       </c>
       <c r="K11">
         <v>322.361342028</v>
@@ -900,10 +966,16 @@
         <v>2.333285819470417</v>
       </c>
       <c r="N11">
-        <v>0.9333143277881668</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>1.166642909735208</v>
+      </c>
+      <c r="O11">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P11">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="2">
         <v>42154</v>
       </c>
@@ -929,10 +1001,10 @@
         <v>3.647969534776978</v>
       </c>
       <c r="I12">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J12">
-        <v>1.459187813910791</v>
+        <v>1.823984767388489</v>
       </c>
       <c r="K12">
         <v>527.2448059755</v>
@@ -944,10 +1016,16 @@
         <v>3.617123928091082</v>
       </c>
       <c r="N12">
-        <v>1.446849571236433</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>1.808561964045541</v>
+      </c>
+      <c r="O12">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P12">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="2">
         <v>42155</v>
       </c>
@@ -973,10 +1051,10 @@
         <v>1.225754796555241</v>
       </c>
       <c r="I13">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J13">
-        <v>0.4903019186220964</v>
+        <v>0.6128773982776204</v>
       </c>
       <c r="K13">
         <v>141.075682452</v>
@@ -988,10 +1066,16 @@
         <v>1.217363200664442</v>
       </c>
       <c r="N13">
-        <v>0.4869452802657769</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>0.6086816003322211</v>
+      </c>
+      <c r="O13">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P13">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="2">
         <v>42156</v>
       </c>
@@ -1017,10 +1101,10 @@
         <v>3.653511431029013</v>
       </c>
       <c r="I14">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J14">
-        <v>1.461404572411605</v>
+        <v>1.826755715514506</v>
       </c>
       <c r="K14">
         <v>550.0758946815</v>
@@ -1032,10 +1116,16 @@
         <v>3.622508447390641</v>
       </c>
       <c r="N14">
-        <v>1.449003378956257</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>1.811254223695321</v>
+      </c>
+      <c r="O14">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P14">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="2">
         <v>42157</v>
       </c>
@@ -1061,10 +1151,10 @@
         <v>2.956426539463806</v>
       </c>
       <c r="I15">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J15">
-        <v>1.182570615785522</v>
+        <v>1.478213269731903</v>
       </c>
       <c r="K15">
         <v>385.913551635</v>
@@ -1076,10 +1166,16 @@
         <v>2.932190619442935</v>
       </c>
       <c r="N15">
-        <v>1.172876247777174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>1.466095309721468</v>
+      </c>
+      <c r="O15">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P15">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="2">
         <v>42158</v>
       </c>
@@ -1105,10 +1201,10 @@
         <v>2.911153101821258</v>
       </c>
       <c r="I16">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J16">
-        <v>1.164461240728503</v>
+        <v>1.455576550910629</v>
       </c>
       <c r="K16">
         <v>373.816482246</v>
@@ -1120,10 +1216,16 @@
         <v>2.88737585445543</v>
       </c>
       <c r="N16">
-        <v>1.154950341782172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>1.443687927227715</v>
+      </c>
+      <c r="O16">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P16">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="2">
         <v>42159</v>
       </c>
@@ -1149,10 +1251,10 @@
         <v>5.147418543063888</v>
       </c>
       <c r="I17">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J17">
-        <v>2.058967417225555</v>
+        <v>2.573709271531944</v>
       </c>
       <c r="K17">
         <v>673.2615449384999</v>
@@ -1164,10 +1266,16 @@
         <v>5.103068151884762</v>
       </c>
       <c r="N17">
-        <v>2.041227260753905</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>2.551534075942381</v>
+      </c>
+      <c r="O17">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P17">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="2">
         <v>42160</v>
       </c>
@@ -1193,10 +1301,10 @@
         <v>5.004562412915388</v>
       </c>
       <c r="I18">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J18">
-        <v>2.001824965166155</v>
+        <v>2.502281206457694</v>
       </c>
       <c r="K18">
         <v>585.8559590714999</v>
@@ -1208,10 +1316,16 @@
         <v>4.961879312861077</v>
       </c>
       <c r="N18">
-        <v>1.984751725144431</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>2.480939656430539</v>
+      </c>
+      <c r="O18">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P18">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="2">
         <v>42161</v>
       </c>
@@ -1237,10 +1351,10 @@
         <v>4.998201313246128</v>
       </c>
       <c r="I19">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J19">
-        <v>1.999280525298451</v>
+        <v>2.499100656623064</v>
       </c>
       <c r="K19">
         <v>678.287792079</v>
@@ -1252,10 +1366,16 @@
         <v>4.955114702389479</v>
       </c>
       <c r="N19">
-        <v>1.982045880955792</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>2.47755735119474</v>
+      </c>
+      <c r="O19">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P19">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="2">
         <v>42162</v>
       </c>
@@ -1281,10 +1401,10 @@
         <v>4.931873749031412</v>
       </c>
       <c r="I20">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J20">
-        <v>1.972749499612565</v>
+        <v>2.465936874515706</v>
       </c>
       <c r="K20">
         <v>689.873717691</v>
@@ -1296,10 +1416,16 @@
         <v>4.889310257333615</v>
       </c>
       <c r="N20">
-        <v>1.955724102933446</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>2.444655128666807</v>
+      </c>
+      <c r="O20">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P20">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="2">
         <v>42163</v>
       </c>
@@ -1325,10 +1451,10 @@
         <v>4.91364289</v>
       </c>
       <c r="I21">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J21">
-        <v>1.965457156</v>
+        <v>2.456821445</v>
       </c>
       <c r="K21">
         <v>699.415068195</v>
@@ -1340,10 +1466,16 @@
         <v>4.8711979432675</v>
       </c>
       <c r="N21">
-        <v>1.948479177307</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>2.43559897163375</v>
+      </c>
+      <c r="O21">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P21">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="2">
         <v>42164</v>
       </c>
@@ -1369,10 +1501,10 @@
         <v>3.528055639110801</v>
       </c>
       <c r="I22">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J22">
-        <v>1.411222255644321</v>
+        <v>1.764027819555401</v>
       </c>
       <c r="K22">
         <v>490.7832165495</v>
@@ -1384,10 +1516,16 @@
         <v>3.498413110912884</v>
       </c>
       <c r="N22">
-        <v>1.399365244365153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>1.749206555456442</v>
+      </c>
+      <c r="O22">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P22">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="2">
         <v>42165</v>
       </c>
@@ -1413,10 +1551,10 @@
         <v>3.805151946720811</v>
       </c>
       <c r="I23">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J23">
-        <v>1.522060778688324</v>
+        <v>1.902575973360406</v>
       </c>
       <c r="K23">
         <v>496.1502262079999</v>
@@ -1428,10 +1566,16 @@
         <v>3.773149532330395</v>
       </c>
       <c r="N23">
-        <v>1.509259812932158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>1.886574766165197</v>
+      </c>
+      <c r="O23">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P23">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="2">
         <v>42166</v>
       </c>
@@ -1457,10 +1601,10 @@
         <v>5.415104319905465</v>
       </c>
       <c r="I24">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J24">
-        <v>2.166041727962186</v>
+        <v>2.707552159952733</v>
       </c>
       <c r="K24">
         <v>648.8118342720001</v>
@@ -1472,10 +1616,16 @@
         <v>5.368567725330387</v>
       </c>
       <c r="N24">
-        <v>2.147427090132155</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>2.684283862665194</v>
+      </c>
+      <c r="O24">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P24">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="2">
         <v>42167</v>
       </c>
@@ -1501,10 +1651,10 @@
         <v>4.182467342317297</v>
       </c>
       <c r="I25">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J25">
-        <v>1.672986936926919</v>
+        <v>2.091233671158649</v>
       </c>
       <c r="K25">
         <v>490.1868821429999</v>
@@ -1516,10 +1666,16 @@
         <v>4.147330402205365</v>
       </c>
       <c r="N25">
-        <v>1.658932160882146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>2.073665201102683</v>
+      </c>
+      <c r="O25">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P25">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="2">
         <v>42168</v>
       </c>
@@ -1545,10 +1701,10 @@
         <v>5.141366360600577</v>
       </c>
       <c r="I26">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J26">
-        <v>2.056546544240231</v>
+        <v>2.570683180300288</v>
       </c>
       <c r="K26">
         <v>641.655821394</v>
@@ -1560,10 +1716,16 @@
         <v>5.097217155355012</v>
       </c>
       <c r="N26">
-        <v>2.038886862142005</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>2.548608577677506</v>
+      </c>
+      <c r="O26">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P26">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="2">
         <v>42169</v>
       </c>
@@ -1589,10 +1751,10 @@
         <v>3.317083670912442</v>
       </c>
       <c r="I27">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J27">
-        <v>1.326833468364977</v>
+        <v>1.658541835456221</v>
       </c>
       <c r="K27">
         <v>408.744640341</v>
@@ -1604,10 +1766,16 @@
         <v>3.289717294421941</v>
       </c>
       <c r="N27">
-        <v>1.315886917768776</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>1.64485864721097</v>
+      </c>
+      <c r="O27">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P27">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="2">
         <v>42170</v>
       </c>
@@ -1633,10 +1801,10 @@
         <v>2.672152251997435</v>
       </c>
       <c r="I28">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J28">
-        <v>1.068860900798974</v>
+        <v>1.336076125998718</v>
       </c>
       <c r="K28">
         <v>328.7506392405</v>
@@ -1648,10 +1816,16 @@
         <v>2.650671631945505</v>
       </c>
       <c r="N28">
-        <v>1.060268652778202</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>1.325335815972752</v>
+      </c>
+      <c r="O28">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P28">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="2">
         <v>42171</v>
       </c>
@@ -1677,10 +1851,10 @@
         <v>4.828613736517887</v>
       </c>
       <c r="I29">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J29">
-        <v>1.931445494607155</v>
+        <v>2.414306868258944</v>
       </c>
       <c r="K29">
         <v>647.108021682</v>
@@ -1692,10 +1866,16 @@
         <v>4.787125102896324</v>
       </c>
       <c r="N29">
-        <v>1.91485004115853</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>2.393562551448162</v>
+      </c>
+      <c r="O29">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P29">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="2">
         <v>42172</v>
       </c>
@@ -1721,10 +1901,10 @@
         <v>4.578591065334181</v>
       </c>
       <c r="I30">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J30">
-        <v>1.831436426133672</v>
+        <v>2.289295532667091</v>
       </c>
       <c r="K30">
         <v>594.63059391</v>
@@ -1736,10 +1916,16 @@
         <v>4.539496028279013</v>
       </c>
       <c r="N30">
-        <v>1.815798411311605</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>2.269748014139506</v>
+      </c>
+      <c r="O30">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P30">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="2">
         <v>42173</v>
       </c>
@@ -1765,10 +1951,10 @@
         <v>1.216288916311688</v>
       </c>
       <c r="I31">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J31">
-        <v>0.4865155665246753</v>
+        <v>0.6081444581558441</v>
       </c>
       <c r="K31">
         <v>124.548700329</v>
@@ -1780,10 +1966,16 @@
         <v>1.208239704874766</v>
       </c>
       <c r="N31">
-        <v>0.4832958819499064</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>0.604119852437383</v>
+      </c>
+      <c r="O31">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P31">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="2">
         <v>42174</v>
       </c>
@@ -1809,10 +2001,10 @@
         <v>4.262775192348291</v>
       </c>
       <c r="I32">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J32">
-        <v>1.705110076939317</v>
+        <v>2.131387596174146</v>
       </c>
       <c r="K32">
         <v>577.933230528</v>
@@ -1824,10 +2016,16 @@
         <v>4.226457490673726</v>
       </c>
       <c r="N32">
-        <v>1.69058299626949</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>2.113228745336863</v>
+      </c>
+      <c r="O32">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P32">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="2">
         <v>42175</v>
       </c>
@@ -1853,10 +2051,10 @@
         <v>2.632972042691943</v>
       </c>
       <c r="I33">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J33">
-        <v>1.053188817076777</v>
+        <v>1.316486021345971</v>
       </c>
       <c r="K33">
         <v>331.9026925319999</v>
@@ -1868,10 +2066,16 @@
         <v>2.611780025230692</v>
       </c>
       <c r="N33">
-        <v>1.044712010092277</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>1.305890012615346</v>
+      </c>
+      <c r="O33">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P33">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="2">
         <v>42176</v>
       </c>
@@ -1897,10 +2101,10 @@
         <v>3.174245326051967</v>
       </c>
       <c r="I34">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J34">
-        <v>2.221971728236377</v>
+        <v>3.174245326051967</v>
       </c>
       <c r="K34">
         <v>397.2439053584999</v>
@@ -1912,10 +2116,16 @@
         <v>3.148139083152055</v>
       </c>
       <c r="N34">
-        <v>2.203697358206438</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>3.148139083152055</v>
+      </c>
+      <c r="O34">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P34">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="2">
         <v>42177</v>
       </c>
@@ -1941,10 +2151,10 @@
         <v>1.420815618775717</v>
       </c>
       <c r="I35">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J35">
-        <v>0.9945709331430016</v>
+        <v>1.420815618775717</v>
       </c>
       <c r="K35">
         <v>169.6145433345</v>
@@ -1956,10 +2166,16 @@
         <v>1.410643837371181</v>
       </c>
       <c r="N35">
-        <v>0.9874506861598269</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>1.410643837371181</v>
+      </c>
+      <c r="O35">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P35">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="2">
         <v>42178</v>
       </c>
@@ -1985,10 +2201,10 @@
         <v>3.213803661164329</v>
       </c>
       <c r="I36">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J36">
-        <v>2.24966256281503</v>
+        <v>3.213803661164329</v>
       </c>
       <c r="K36">
         <v>445.035848508</v>
@@ -2000,10 +2216,16 @@
         <v>3.187053564230696</v>
       </c>
       <c r="N36">
-        <v>2.230937494961487</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+        <v>3.187053564230696</v>
+      </c>
+      <c r="O36">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P36">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="2">
         <v>42179</v>
       </c>
@@ -2029,10 +2251,10 @@
         <v>4.590574736959907</v>
       </c>
       <c r="I37">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J37">
-        <v>3.213402315871935</v>
+        <v>4.590574736959907</v>
       </c>
       <c r="K37">
         <v>606.9832351875</v>
@@ -2044,10 +2266,16 @@
         <v>4.551315934850892</v>
       </c>
       <c r="N37">
-        <v>3.185921154395624</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+        <v>4.551315934850892</v>
+      </c>
+      <c r="O37">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P37">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" s="2">
         <v>42180</v>
       </c>
@@ -2073,10 +2301,10 @@
         <v>5.490493998484458</v>
       </c>
       <c r="I38">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J38">
-        <v>3.84334579893912</v>
+        <v>5.490493998484458</v>
       </c>
       <c r="K38">
         <v>665.0832445065</v>
@@ -2088,10 +2316,16 @@
         <v>5.443227487943906</v>
       </c>
       <c r="N38">
-        <v>3.810259241560734</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+        <v>5.443227487943906</v>
+      </c>
+      <c r="O38">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P38">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="2">
         <v>42181</v>
       </c>
@@ -2117,10 +2351,10 @@
         <v>5.21362653056338</v>
       </c>
       <c r="I39">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J39">
-        <v>3.649538571394366</v>
+        <v>5.21362653056338</v>
       </c>
       <c r="K39">
         <v>601.8717974175</v>
@@ -2132,10 +2366,16 @@
         <v>5.169067914733134</v>
       </c>
       <c r="N39">
-        <v>3.618347540313193</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>5.169067914733134</v>
+      </c>
+      <c r="O39">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P39">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="2">
         <v>42182</v>
       </c>
@@ -2161,10 +2401,10 @@
         <v>4.490837873409825</v>
       </c>
       <c r="I40">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J40">
-        <v>3.143586511386878</v>
+        <v>4.490837873409825</v>
       </c>
       <c r="K40">
         <v>551.183372865</v>
@@ -2176,10 +2416,16 @@
         <v>4.452723174353642</v>
       </c>
       <c r="N40">
-        <v>3.116906222047549</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+        <v>4.452723174353642</v>
+      </c>
+      <c r="O40">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P40">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" s="2">
         <v>42183</v>
       </c>
@@ -2205,10 +2451,10 @@
         <v>5.532581356981726</v>
       </c>
       <c r="I41">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J41">
-        <v>3.872806949887208</v>
+        <v>5.532581356981726</v>
       </c>
       <c r="K41">
         <v>669.6835384994999</v>
@@ -2220,10 +2466,16 @@
         <v>5.48492983433138</v>
       </c>
       <c r="N41">
-        <v>3.839450884031966</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+        <v>5.48492983433138</v>
+      </c>
+      <c r="O41">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P41">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="2">
         <v>42184</v>
       </c>
@@ -2249,10 +2501,10 @@
         <v>5.612106909410137</v>
       </c>
       <c r="I42">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J42">
-        <v>3.928474836587096</v>
+        <v>5.612106909410137</v>
       </c>
       <c r="K42">
         <v>681.2694641115</v>
@@ -2264,10 +2516,16 @@
         <v>5.563713756903624</v>
       </c>
       <c r="N42">
-        <v>3.894599629832537</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+        <v>5.563713756903624</v>
+      </c>
+      <c r="O42">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P42">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" s="2">
         <v>42185</v>
       </c>
@@ -2293,10 +2551,10 @@
         <v>6.021827360563409</v>
       </c>
       <c r="I43">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J43">
-        <v>4.215279152394387</v>
+        <v>6.021827360563409</v>
       </c>
       <c r="K43">
         <v>690.4700520975</v>
@@ -2308,10 +2566,16 @@
         <v>5.969854247834814</v>
       </c>
       <c r="N43">
-        <v>4.17889797348437</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+        <v>5.969854247834814</v>
+      </c>
+      <c r="O43">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P43">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" s="2">
         <v>42186</v>
       </c>
@@ -2337,10 +2601,10 @@
         <v>6.233663307966014</v>
       </c>
       <c r="I44">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J44">
-        <v>4.36356431557621</v>
+        <v>6.233663307966014</v>
       </c>
       <c r="K44">
         <v>670.109491647</v>
@@ -2352,10 +2616,16 @@
         <v>6.179971091866054</v>
       </c>
       <c r="N44">
-        <v>4.325979764306238</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
+        <v>6.179971091866054</v>
+      </c>
+      <c r="O44">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P44">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" s="2">
         <v>42187</v>
       </c>
@@ -2381,10 +2651,10 @@
         <v>5.111098212268947</v>
       </c>
       <c r="I45">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J45">
-        <v>3.577768748588263</v>
+        <v>5.111098212268947</v>
       </c>
       <c r="K45">
         <v>565.5805892505</v>
@@ -2396,10 +2666,16 @@
         <v>5.067627980455828</v>
       </c>
       <c r="N45">
-        <v>3.547339586319079</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+        <v>5.067627980455828</v>
+      </c>
+      <c r="O45">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P45">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" s="2">
         <v>42188</v>
       </c>
@@ -2425,10 +2701,10 @@
         <v>5.873929954059493</v>
       </c>
       <c r="I46">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J46">
-        <v>4.111750967841645</v>
+        <v>5.873929954059493</v>
       </c>
       <c r="K46">
         <v>653.241747006</v>
@@ -2440,10 +2716,16 @@
         <v>5.823425986274047</v>
       </c>
       <c r="N46">
-        <v>4.076398190391832</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+        <v>5.823425986274047</v>
+      </c>
+      <c r="O46">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P46">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" s="2">
         <v>42189</v>
       </c>
@@ -2469,10 +2751,10 @@
         <v>5.445451756425532</v>
       </c>
       <c r="I47">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J47">
-        <v>3.811816229497872</v>
+        <v>5.445451756425532</v>
       </c>
       <c r="K47">
         <v>587.1338185139999</v>
@@ -2484,10 +2766,16 @@
         <v>5.399000500792716</v>
       </c>
       <c r="N47">
-        <v>3.779300350554901</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>5.399000500792716</v>
+      </c>
+      <c r="O47">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P47">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" s="2">
         <v>42190</v>
       </c>
@@ -2513,10 +2801,10 @@
         <v>3.682617488658199</v>
       </c>
       <c r="I48">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J48">
-        <v>2.577832242060739</v>
+        <v>3.682617488658199</v>
       </c>
       <c r="K48">
         <v>421.863997284</v>
@@ -2528,10 +2816,16 @@
         <v>3.652132934356921</v>
       </c>
       <c r="N48">
-        <v>2.556493054049844</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+        <v>3.652132934356921</v>
+      </c>
+      <c r="O48">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P48">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49" s="2">
         <v>42191</v>
       </c>
@@ -2557,10 +2851,10 @@
         <v>5.570876841048149</v>
       </c>
       <c r="I49">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J49">
-        <v>3.899613788733704</v>
+        <v>5.570876841048149</v>
       </c>
       <c r="K49">
         <v>658.4383754055</v>
@@ -2572,10 +2866,16 @@
         <v>5.522951858256888</v>
       </c>
       <c r="N49">
-        <v>3.866066300779821</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+        <v>5.522951858256888</v>
+      </c>
+      <c r="O49">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P49">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50" s="2">
         <v>42192</v>
       </c>
@@ -2601,10 +2901,10 @@
         <v>4.347923557525038</v>
       </c>
       <c r="I50">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J50">
-        <v>3.043546490267527</v>
+        <v>4.347923557525038</v>
       </c>
       <c r="K50">
         <v>496.9169418735</v>
@@ -2616,10 +2916,16 @@
         <v>4.311351156264553</v>
       </c>
       <c r="N50">
-        <v>3.017945809385187</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+        <v>4.311351156264553</v>
+      </c>
+      <c r="O50">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P50">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51" s="2">
         <v>42193</v>
       </c>
@@ -2645,10 +2951,10 @@
         <v>2.48587168038806</v>
       </c>
       <c r="I51">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J51">
-        <v>1.740110176271642</v>
+        <v>2.48587168038806</v>
       </c>
       <c r="K51">
         <v>300.8081127645</v>
@@ -2660,10 +2966,16 @@
         <v>2.466128673314619</v>
       </c>
       <c r="N51">
-        <v>1.726290071320234</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
+        <v>2.466128673314619</v>
+      </c>
+      <c r="O51">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P51">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" s="2">
         <v>42194</v>
       </c>
@@ -2689,10 +3001,10 @@
         <v>3.965591222542951</v>
       </c>
       <c r="I52">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J52">
-        <v>2.775913855780066</v>
+        <v>3.965591222542951</v>
       </c>
       <c r="K52">
         <v>508.9288206329999</v>
@@ -2704,10 +3016,16 @@
         <v>3.932163273171085</v>
       </c>
       <c r="N52">
-        <v>2.75251429121976</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+        <v>3.932163273171085</v>
+      </c>
+      <c r="O52">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P52">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" s="2">
         <v>42195</v>
       </c>
@@ -2733,10 +3051,10 @@
         <v>5.550575166714903</v>
       </c>
       <c r="I53">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J53">
-        <v>3.885402616700432</v>
+        <v>5.550575166714903</v>
       </c>
       <c r="K53">
         <v>694.2184397955001</v>
@@ -2748,10 +3066,16 @@
         <v>5.502652009815219</v>
       </c>
       <c r="N53">
-        <v>3.851856406870653</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+        <v>5.502652009815219</v>
+      </c>
+      <c r="O53">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P53">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" s="2">
         <v>42196</v>
       </c>
@@ -2777,10 +3101,10 @@
         <v>5.614380604568507</v>
       </c>
       <c r="I54">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J54">
-        <v>3.930066423197955</v>
+        <v>5.614380604568507</v>
       </c>
       <c r="K54">
         <v>674.4542137515</v>
@@ -2792,10 +3116,16 @@
         <v>5.566000983771749</v>
       </c>
       <c r="N54">
-        <v>3.896200688640224</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
+        <v>5.566000983771749</v>
+      </c>
+      <c r="O54">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P54">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" s="2">
         <v>42197</v>
       </c>
@@ -2821,10 +3151,10 @@
         <v>3.468582965786408</v>
       </c>
       <c r="I55">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J55">
-        <v>2.428008076050485</v>
+        <v>3.468582965786408</v>
       </c>
       <c r="K55">
         <v>419.9046128055</v>
@@ -2836,10 +3166,16 @@
         <v>3.439884252964534</v>
       </c>
       <c r="N55">
-        <v>2.407918977075174</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14">
+        <v>3.439884252964534</v>
+      </c>
+      <c r="O55">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P55">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56" s="2">
         <v>42198</v>
       </c>
@@ -2865,10 +3201,10 @@
         <v>2.28118472798784</v>
       </c>
       <c r="I56">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J56">
-        <v>1.596829309591488</v>
+        <v>2.28118472798784</v>
       </c>
       <c r="K56">
         <v>246.6268724025</v>
@@ -2880,10 +3216,16 @@
         <v>2.263613190212998</v>
       </c>
       <c r="N56">
-        <v>1.584529233149098</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
+        <v>2.263613190212998</v>
+      </c>
+      <c r="O56">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P56">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57" s="2">
         <v>42199</v>
       </c>
@@ -2909,10 +3251,10 @@
         <v>3.176639476971981</v>
       </c>
       <c r="I57">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J57">
-        <v>2.223647633880387</v>
+        <v>3.176639476971981</v>
       </c>
       <c r="K57">
         <v>364.3603223715</v>
@@ -2924,10 +3266,16 @@
         <v>3.150772385573394</v>
       </c>
       <c r="N57">
-        <v>2.205540669901376</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
+        <v>3.150772385573394</v>
+      </c>
+      <c r="O57">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P57">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58" s="2">
         <v>42200</v>
       </c>
@@ -2953,10 +3301,10 @@
         <v>4.236812068812003</v>
       </c>
       <c r="I58">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J58">
-        <v>2.965768448168402</v>
+        <v>4.236812068812003</v>
       </c>
       <c r="K58">
         <v>486.097731927</v>
@@ -2968,10 +3316,16 @@
         <v>4.201246038640629</v>
       </c>
       <c r="N58">
-        <v>2.94087222704844</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14">
+        <v>4.201246038640629</v>
+      </c>
+      <c r="O58">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P58">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59" s="2">
         <v>42201</v>
       </c>
@@ -2997,10 +3351,10 @@
         <v>5.893015619857835</v>
       </c>
       <c r="I59">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J59">
-        <v>4.125110933900484</v>
+        <v>5.893015619857835</v>
       </c>
       <c r="K59">
         <v>656.0530377795</v>
@@ -3012,10 +3366,16 @@
         <v>5.842332244760255</v>
       </c>
       <c r="N59">
-        <v>4.089632571332179</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14">
+        <v>5.842332244760255</v>
+      </c>
+      <c r="O59">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P59">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60" s="2">
         <v>42202</v>
       </c>
@@ -3041,10 +3401,10 @@
         <v>4.83811494187258</v>
       </c>
       <c r="I60">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J60">
-        <v>3.386680459310806</v>
+        <v>4.83811494187258</v>
       </c>
       <c r="K60">
         <v>540.1937816595001</v>
@@ -3056,10 +3416,16 @@
         <v>4.797121599459759</v>
       </c>
       <c r="N60">
-        <v>3.357985119621831</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+        <v>4.797121599459759</v>
+      </c>
+      <c r="O60">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P60">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61" s="2">
         <v>42203</v>
       </c>
@@ -3085,10 +3451,10 @@
         <v>4.260784952088116</v>
       </c>
       <c r="I61">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J61">
-        <v>2.982549466461681</v>
+        <v>4.260784952088116</v>
       </c>
       <c r="K61">
         <v>492.1462666215</v>
@@ -3100,10 +3466,16 @@
         <v>4.224976980333372</v>
       </c>
       <c r="N61">
-        <v>2.95748388623336</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
+        <v>4.224976980333372</v>
+      </c>
+      <c r="O61">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P61">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" s="2">
         <v>42204</v>
       </c>
@@ -3129,10 +3501,10 @@
         <v>3.230182557987347</v>
       </c>
       <c r="I62">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J62">
-        <v>2.261127790591143</v>
+        <v>3.230182557987347</v>
       </c>
       <c r="K62">
         <v>365.3826099255</v>
@@ -3144,10 +3516,16 @@
         <v>3.203870659203958</v>
       </c>
       <c r="N62">
-        <v>2.24270946144277</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14">
+        <v>3.203870659203958</v>
+      </c>
+      <c r="O62">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P62">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63" s="2">
         <v>42205</v>
       </c>
@@ -3173,10 +3551,10 @@
         <v>1.701185052682019</v>
       </c>
       <c r="I63">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J63">
-        <v>1.190829536877414</v>
+        <v>1.701185052682019</v>
       </c>
       <c r="K63">
         <v>166.0365368955</v>
@@ -3188,10 +3566,16 @@
         <v>1.689065111759591</v>
       </c>
       <c r="N63">
-        <v>1.182345578231714</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
+        <v>1.689065111759591</v>
+      </c>
+      <c r="O63">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P63">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64" s="2">
         <v>42206</v>
       </c>
@@ -3217,10 +3601,10 @@
         <v>3.243844972222318</v>
       </c>
       <c r="I64">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J64">
-        <v>2.919460475000086</v>
+        <v>3.243844972222318</v>
       </c>
       <c r="K64">
         <v>356.267212569</v>
@@ -3232,10 +3616,16 @@
         <v>3.217502253602254</v>
       </c>
       <c r="N64">
-        <v>2.895752028242028</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14">
+        <v>3.217502253602254</v>
+      </c>
+      <c r="O64">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P64">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65" s="2">
         <v>42207</v>
       </c>
@@ -3261,10 +3651,10 @@
         <v>3.7680707424912</v>
       </c>
       <c r="I65">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J65">
-        <v>3.39126366824208</v>
+        <v>3.7680707424912</v>
       </c>
       <c r="K65">
         <v>436.17602304</v>
@@ -3276,10 +3666,16 @@
         <v>3.736770884024144</v>
       </c>
       <c r="N65">
-        <v>3.36309379562173</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
+        <v>3.736770884024144</v>
+      </c>
+      <c r="O65">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P65">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66" s="2">
         <v>42208</v>
       </c>
@@ -3305,10 +3701,10 @@
         <v>4.406595458858659</v>
       </c>
       <c r="I66">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J66">
-        <v>3.965935912972793</v>
+        <v>4.406595458858659</v>
       </c>
       <c r="K66">
         <v>533.8896750765</v>
@@ -3320,10 +3716,16 @@
         <v>4.369295377128509</v>
       </c>
       <c r="N66">
-        <v>3.932365839415658</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14">
+        <v>4.369295377128509</v>
+      </c>
+      <c r="O66">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P66">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67" s="2">
         <v>42209</v>
       </c>
@@ -3349,10 +3751,10 @@
         <v>3.815344467147541</v>
       </c>
       <c r="I67">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J67">
-        <v>3.433810020432787</v>
+        <v>3.815344467147541</v>
       </c>
       <c r="K67">
         <v>443.161654659</v>
@@ -3364,10 +3766,16 @@
         <v>3.783600891482163</v>
       </c>
       <c r="N67">
-        <v>3.405240802333947</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14">
+        <v>3.783600891482163</v>
+      </c>
+      <c r="O67">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P67">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68" s="2">
         <v>42210</v>
       </c>
@@ -3393,10 +3801,10 @@
         <v>3.47187957386848</v>
       </c>
       <c r="I68">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J68">
-        <v>3.124691616481632</v>
+        <v>3.47187957386848</v>
       </c>
       <c r="K68">
         <v>434.642591709</v>
@@ -3408,10 +3816,16 @@
         <v>3.443050430440582</v>
       </c>
       <c r="N68">
-        <v>3.098745387396524</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14">
+        <v>3.443050430440582</v>
+      </c>
+      <c r="O68">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P68">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69" s="2">
         <v>42211</v>
       </c>
@@ -3437,10 +3851,10 @@
         <v>1.682421419969681</v>
       </c>
       <c r="I69">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J69">
-        <v>1.514179277972713</v>
+        <v>1.682421419969681</v>
       </c>
       <c r="K69">
         <v>200.538741843</v>
@@ -3452,10 +3866,16 @@
         <v>1.669941770887479</v>
       </c>
       <c r="N69">
-        <v>1.502947593798731</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14">
+        <v>1.669941770887479</v>
+      </c>
+      <c r="O69">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P69">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
       <c r="A70" s="2">
         <v>42212</v>
       </c>
@@ -3481,10 +3901,10 @@
         <v>2.587351594601051</v>
       </c>
       <c r="I70">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J70">
-        <v>2.328616435140946</v>
+        <v>2.587351594601051</v>
       </c>
       <c r="K70">
         <v>309.4975569735</v>
@@ -3496,10 +3916,16 @@
         <v>2.56672072420674</v>
       </c>
       <c r="N70">
-        <v>2.310048651786066</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14">
+        <v>2.56672072420674</v>
+      </c>
+      <c r="O70">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P70">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
       <c r="A71" s="2">
         <v>42213</v>
       </c>
@@ -3525,10 +3951,10 @@
         <v>2.269824082630849</v>
       </c>
       <c r="I71">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J71">
-        <v>2.042841674367764</v>
+        <v>2.269824082630849</v>
       </c>
       <c r="K71">
         <v>283.0884618285</v>
@@ -3540,10 +3966,16 @@
         <v>2.251955094615214</v>
       </c>
       <c r="N71">
-        <v>2.026759585153693</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14">
+        <v>2.251955094615214</v>
+      </c>
+      <c r="O71">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P71">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
       <c r="A72" s="2">
         <v>42214</v>
       </c>
@@ -3569,10 +4001,10 @@
         <v>3.264805944405549</v>
       </c>
       <c r="I72">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J72">
-        <v>2.938325349964995</v>
+        <v>3.264805944405549</v>
       </c>
       <c r="K72">
         <v>429.190391421</v>
@@ -3584,10 +4016,16 @@
         <v>3.237731449398453</v>
       </c>
       <c r="N72">
-        <v>2.913958304458608</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14">
+        <v>3.237731449398453</v>
+      </c>
+      <c r="O72">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P72">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
       <c r="A73" s="2">
         <v>42215</v>
       </c>
@@ -3613,10 +4051,10 @@
         <v>3.535967891447941</v>
       </c>
       <c r="I73">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J73">
-        <v>3.182371102303147</v>
+        <v>3.535967891447941</v>
       </c>
       <c r="K73">
         <v>472.9783749840001</v>
@@ -3628,10 +4066,16 @@
         <v>3.506361066176019</v>
       </c>
       <c r="N73">
-        <v>3.155724959558417</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14">
+        <v>3.506361066176019</v>
+      </c>
+      <c r="O73">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P73">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
       <c r="A74" s="2">
         <v>42216</v>
       </c>
@@ -3657,10 +4101,10 @@
         <v>4.506046117768801</v>
       </c>
       <c r="I74">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="J74">
-        <v>4.731348423657241</v>
+        <v>4.506046117768801</v>
       </c>
       <c r="K74">
         <v>608.772238407</v>
@@ -3672,10 +4116,16 @@
         <v>4.467501661415954</v>
       </c>
       <c r="N74">
-        <v>4.690876744486752</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14">
+        <v>4.467501661415954</v>
+      </c>
+      <c r="O74">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P74">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
       <c r="A75" s="2">
         <v>42217</v>
       </c>
@@ -3701,10 +4151,10 @@
         <v>4.929732026182196</v>
       </c>
       <c r="I75">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="J75">
-        <v>5.176218627491306</v>
+        <v>4.929732026182196</v>
       </c>
       <c r="K75">
         <v>622.3175484975</v>
@@ -3716,10 +4166,16 @@
         <v>4.887494204952255</v>
       </c>
       <c r="N75">
-        <v>5.131868915199868</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14">
+        <v>4.887494204952255</v>
+      </c>
+      <c r="O75">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P75">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
       <c r="A76" s="2">
         <v>42218</v>
       </c>
@@ -3745,10 +4201,10 @@
         <v>5.233516609375464</v>
       </c>
       <c r="I76">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="J76">
-        <v>5.495192439844237</v>
+        <v>5.233516609375464</v>
       </c>
       <c r="K76">
         <v>636.033239847</v>
@@ -3760,10 +4216,16 @@
         <v>5.188604559363276</v>
       </c>
       <c r="N76">
-        <v>5.448034787331441</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14">
+        <v>5.188604559363276</v>
+      </c>
+      <c r="O76">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P76">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77" s="2">
         <v>42219</v>
       </c>
@@ -3806,8 +4268,14 @@
       <c r="N77">
         <v>5.31367305598834</v>
       </c>
-    </row>
-    <row r="78" spans="1:14">
+      <c r="O77">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P77">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78" s="2">
         <v>42220</v>
       </c>
@@ -3850,8 +4318,14 @@
       <c r="N78">
         <v>4.22040213010011</v>
       </c>
-    </row>
-    <row r="79" spans="1:14">
+      <c r="O78">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P78">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
       <c r="A79" s="2">
         <v>42221</v>
       </c>
@@ -3894,8 +4368,14 @@
       <c r="N79">
         <v>4.885315833561844</v>
       </c>
-    </row>
-    <row r="80" spans="1:14">
+      <c r="O79">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P79">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80" s="2">
         <v>42222</v>
       </c>
@@ -3938,8 +4418,14 @@
       <c r="N80">
         <v>5.097731940191111</v>
       </c>
-    </row>
-    <row r="81" spans="1:14">
+      <c r="O80">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P80">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16">
       <c r="A81" s="2">
         <v>42223</v>
       </c>
@@ -3982,8 +4468,14 @@
       <c r="N81">
         <v>4.285121483869872</v>
       </c>
-    </row>
-    <row r="82" spans="1:14">
+      <c r="O81">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P81">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16">
       <c r="A82" s="2">
         <v>42224</v>
       </c>
@@ -4026,8 +4518,14 @@
       <c r="N82">
         <v>3.821142459971757</v>
       </c>
-    </row>
-    <row r="83" spans="1:14">
+      <c r="O82">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P82">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16">
       <c r="A83" s="2">
         <v>42225</v>
       </c>
@@ -4070,8 +4568,14 @@
       <c r="N83">
         <v>1.891360693128664</v>
       </c>
-    </row>
-    <row r="84" spans="1:14">
+      <c r="O83">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P83">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
       <c r="A84" s="2">
         <v>42226</v>
       </c>
@@ -4114,8 +4618,14 @@
       <c r="N84">
         <v>3.965131384195644</v>
       </c>
-    </row>
-    <row r="85" spans="1:14">
+      <c r="O84">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P84">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16">
       <c r="A85" s="2">
         <v>42227</v>
       </c>
@@ -4141,10 +4651,10 @@
         <v>3.929183914695377</v>
       </c>
       <c r="I85">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J85">
-        <v>3.143347131756302</v>
+        <v>2.750428740286764</v>
       </c>
       <c r="K85">
         <v>444.183942213</v>
@@ -4156,10 +4666,16 @@
         <v>3.896485631153042</v>
       </c>
       <c r="N85">
-        <v>3.117188504922434</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14">
+        <v>2.727539941807129</v>
+      </c>
+      <c r="O85">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P85">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16">
       <c r="A86" s="2">
         <v>42228</v>
       </c>
@@ -4185,10 +4701,10 @@
         <v>4.810326849416058</v>
       </c>
       <c r="I86">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J86">
-        <v>3.848261479532847</v>
+        <v>3.367228794591241</v>
       </c>
       <c r="K86">
         <v>527.7559497525</v>
@@ -4200,10 +4716,16 @@
         <v>4.769649482993267</v>
       </c>
       <c r="N86">
-        <v>3.815719586394614</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14">
+        <v>3.338754638095287</v>
+      </c>
+      <c r="O86">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P86">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
       <c r="A87" s="2">
         <v>42229</v>
       </c>
@@ -4229,10 +4751,10 @@
         <v>3.216434633553691</v>
       </c>
       <c r="I87">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J87">
-        <v>2.573147706842953</v>
+        <v>2.251504243487584</v>
       </c>
       <c r="K87">
         <v>344.2553338095</v>
@@ -4244,10 +4766,16 @@
         <v>3.190425293562447</v>
       </c>
       <c r="N87">
-        <v>2.552340234849958</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14">
+        <v>2.233297705493713</v>
+      </c>
+      <c r="O87">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P87">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16">
       <c r="A88" s="2">
         <v>42230</v>
       </c>
@@ -4273,10 +4801,10 @@
         <v>3.112298682032323</v>
       </c>
       <c r="I88">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J88">
-        <v>2.489838945625858</v>
+        <v>2.178609077422626</v>
       </c>
       <c r="K88">
         <v>362.741700411</v>
@@ -4288,10 +4816,16 @@
         <v>3.086969039490127</v>
       </c>
       <c r="N88">
-        <v>2.469575231592102</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14">
+        <v>2.160878327643089</v>
+      </c>
+      <c r="O88">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P88">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16">
       <c r="A89" s="2">
         <v>42231</v>
       </c>
@@ -4317,10 +4851,10 @@
         <v>2.848256959387755</v>
       </c>
       <c r="I89">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J89">
-        <v>2.278605567510204</v>
+        <v>1.993779871571429</v>
       </c>
       <c r="K89">
         <v>351.837299835</v>
@@ -4332,10 +4866,16 @@
         <v>2.825162240676683</v>
       </c>
       <c r="N89">
-        <v>2.260129792541347</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14">
+        <v>1.977613568473678</v>
+      </c>
+      <c r="O89">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P89">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16">
       <c r="A90" s="2">
         <v>42232</v>
       </c>
@@ -4361,10 +4901,10 @@
         <v>2.45454306935363</v>
       </c>
       <c r="I90">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J90">
-        <v>1.963634455482904</v>
+        <v>1.718180148547541</v>
       </c>
       <c r="K90">
         <v>302.3415440955</v>
@@ -4376,10 +4916,16 @@
         <v>2.435034886711524</v>
       </c>
       <c r="N90">
-        <v>1.948027909369219</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14">
+        <v>1.704524420698067</v>
+      </c>
+      <c r="O90">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P90">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16">
       <c r="A91" s="2">
         <v>42233</v>
       </c>
@@ -4405,10 +4951,10 @@
         <v>2.805916298735632</v>
       </c>
       <c r="I91">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J91">
-        <v>2.244733038988506</v>
+        <v>1.964141409114942</v>
       </c>
       <c r="K91">
         <v>346.2999089175</v>
@@ -4420,10 +4966,16 @@
         <v>2.783209705156235</v>
       </c>
       <c r="N91">
-        <v>2.226567764124988</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14">
+        <v>1.948246793609365</v>
+      </c>
+      <c r="O91">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P91">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16">
       <c r="A92" s="2">
         <v>42234</v>
       </c>
@@ -4449,10 +5001,10 @@
         <v>2.768322892725848</v>
       </c>
       <c r="I92">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J92">
-        <v>2.214658314180679</v>
+        <v>1.937826024908094</v>
       </c>
       <c r="K92">
         <v>348.5148652845</v>
@@ -4464,10 +5016,16 @@
         <v>2.745902687952469</v>
       </c>
       <c r="N92">
-        <v>2.196722150361975</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14">
+        <v>1.922131881566728</v>
+      </c>
+      <c r="O92">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P92">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16">
       <c r="A93" s="2">
         <v>42235</v>
       </c>
@@ -4493,10 +5051,10 @@
         <v>3.427480728204379</v>
       </c>
       <c r="I93">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J93">
-        <v>2.741984582563504</v>
+        <v>2.399236509743065</v>
       </c>
       <c r="K93">
         <v>415.219128183</v>
@@ -4508,10 +5066,16 @@
         <v>3.399155819789657</v>
       </c>
       <c r="N93">
-        <v>2.719324655831726</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14">
+        <v>2.37940907385276</v>
+      </c>
+      <c r="O93">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P93">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16">
       <c r="A94" s="2">
         <v>42236</v>
       </c>
@@ -4537,10 +5101,10 @@
         <v>2.185639776345483</v>
       </c>
       <c r="I94">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J94">
-        <v>1.748511821076387</v>
+        <v>1.529947843441838</v>
       </c>
       <c r="K94">
         <v>247.3083974385</v>
@@ -4552,10 +5116,16 @@
         <v>2.168796439634573</v>
       </c>
       <c r="N94">
-        <v>1.735037151707659</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14">
+        <v>1.518157507744201</v>
+      </c>
+      <c r="O94">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P94">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16">
       <c r="A95" s="2">
         <v>42237</v>
       </c>
@@ -4581,10 +5151,10 @@
         <v>4.347460880173629</v>
       </c>
       <c r="I95">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J95">
-        <v>3.477968704138903</v>
+        <v>3.04322261612154</v>
       </c>
       <c r="K95">
         <v>507.6509611905</v>
@@ -4596,10 +5166,16 @@
         <v>4.310822141494359</v>
       </c>
       <c r="N95">
-        <v>3.448657713195487</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14">
+        <v>3.017575499046051</v>
+      </c>
+      <c r="O95">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P95">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16">
       <c r="A96" s="2">
         <v>42238</v>
       </c>
@@ -4625,10 +5201,10 @@
         <v>4.78309551707317</v>
       </c>
       <c r="I96">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J96">
-        <v>3.826476413658536</v>
+        <v>3.348166861951219</v>
       </c>
       <c r="K96">
         <v>548.286891462</v>
@@ -4640,10 +5216,16 @@
         <v>4.742518042076829</v>
       </c>
       <c r="N96">
-        <v>3.794014433661463</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14">
+        <v>3.31976262945378</v>
+      </c>
+      <c r="O96">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P96">
+        <v>1.77371166</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16">
       <c r="A97" s="2">
         <v>42239</v>
       </c>
@@ -4669,10 +5251,10 @@
         <v>2.006372039078385</v>
       </c>
       <c r="I97">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J97">
-        <v>1.605097631262708</v>
+        <v>1.404460427354869</v>
       </c>
       <c r="K97">
         <v>217.576867743</v>
@@ -4684,7 +5266,13 @@
         <v>1.991254932633774</v>
       </c>
       <c r="N97">
-        <v>1.593003946107019</v>
+        <v>1.393878452843642</v>
+      </c>
+      <c r="O97">
+        <v>0.5912372199999999</v>
+      </c>
+      <c r="P97">
+        <v>1.77371166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>